<commit_message>
update Table6 data off
</commit_message>
<xml_diff>
--- a/Data/Result.xlsx
+++ b/Data/Result.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\AL\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC714DF5-D31E-4C1D-9B38-37EEBEEB6337}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5EDA75-FD18-4A46-83E6-32D86A333E4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16380" yWindow="168" windowWidth="26856" windowHeight="12276" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Size" sheetId="3" r:id="rId1"/>
     <sheet name="Question_type" sheetId="9" r:id="rId2"/>
     <sheet name="Opportunity_Prediction" sheetId="6" r:id="rId3"/>
-    <sheet name="Sheet5" sheetId="12" r:id="rId4"/>
-    <sheet name="BKT_parameters" sheetId="7" r:id="rId5"/>
-    <sheet name="Columns" sheetId="2" r:id="rId6"/>
-    <sheet name="Table6_analysis" sheetId="10" r:id="rId7"/>
+    <sheet name="BKT_parameters" sheetId="7" r:id="rId4"/>
+    <sheet name="Columns" sheetId="2" r:id="rId5"/>
+    <sheet name="Table6_analysis" sheetId="10" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="252">
   <si>
     <t>Anon Student Id</t>
   </si>
@@ -804,7 +804,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000000000"/>
-    <numFmt numFmtId="172" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -821,7 +821,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -831,6 +831,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -847,7 +865,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -868,7 +886,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -880,6 +898,12 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6608,6 +6632,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.6978133457865012E-4"/>
+          <c:y val="0.13911150156816196"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13817,7 +13849,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14924,6 +14956,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C5F337-64F8-4CBA-8DBD-136E7C1E957B}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15029,11 +15062,11 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N76" sqref="N76"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15904,7 +15937,7 @@
       <c r="B14" s="15">
         <v>3.8965519999999998</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="18">
         <v>29</v>
       </c>
       <c r="D14" s="16">
@@ -15969,7 +16002,7 @@
       <c r="B15" s="15">
         <v>2.8214290000000002</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="18">
         <v>28</v>
       </c>
       <c r="D15" s="16">
@@ -16687,432 +16720,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5CB2B5-6C5F-47C2-9C35-CC76F709C860}">
-  <dimension ref="A1:E24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20.21875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B1">
-        <v>3.733333</v>
-      </c>
-      <c r="C1">
-        <v>30</v>
-      </c>
-      <c r="D1" s="14">
-        <v>0.65920559999999995</v>
-      </c>
-      <c r="E1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2">
-        <v>5.733333</v>
-      </c>
-      <c r="C2">
-        <v>30</v>
-      </c>
-      <c r="D2" s="14">
-        <v>0.9147708</v>
-      </c>
-      <c r="E2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B3">
-        <v>5.8666669999999996</v>
-      </c>
-      <c r="C3">
-        <v>30</v>
-      </c>
-      <c r="D3" s="14">
-        <v>0.62019329999999995</v>
-      </c>
-      <c r="E3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B4">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="C4">
-        <v>30</v>
-      </c>
-      <c r="D4" s="14">
-        <v>0.83777950000000001</v>
-      </c>
-      <c r="E4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5">
-        <v>9.4</v>
-      </c>
-      <c r="C5">
-        <v>30</v>
-      </c>
-      <c r="D5" s="14">
-        <v>0.54586270000000003</v>
-      </c>
-      <c r="E5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B6">
-        <v>9.233333</v>
-      </c>
-      <c r="C6">
-        <v>30</v>
-      </c>
-      <c r="D6" s="14">
-        <v>0.57153419999999999</v>
-      </c>
-      <c r="E6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7">
-        <v>2.6071430000000002</v>
-      </c>
-      <c r="C7">
-        <v>28</v>
-      </c>
-      <c r="D7" s="14">
-        <v>0.85609900000000005</v>
-      </c>
-      <c r="E7">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B8">
-        <v>6.3333329999999997</v>
-      </c>
-      <c r="C8">
-        <v>30</v>
-      </c>
-      <c r="D8" s="14">
-        <v>0.99174839999999997</v>
-      </c>
-      <c r="E8">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>117</v>
-      </c>
-      <c r="B9">
-        <v>1.0769230000000001</v>
-      </c>
-      <c r="C9">
-        <v>13</v>
-      </c>
-      <c r="D9" s="14">
-        <v>9.2487780000000004E-10</v>
-      </c>
-      <c r="E9">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>118</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>8</v>
-      </c>
-      <c r="D10" s="14">
-        <v>8.4851119999999999E-35</v>
-      </c>
-      <c r="E10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>119</v>
-      </c>
-      <c r="B11">
-        <v>1.3333330000000001</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11" s="14">
-        <v>1.439073E-144</v>
-      </c>
-      <c r="E11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12" s="14">
-        <v>2.209427E-218</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>121</v>
-      </c>
-      <c r="B13">
-        <v>4.3666669999999996</v>
-      </c>
-      <c r="C13">
-        <v>30</v>
-      </c>
-      <c r="D13" s="14">
-        <v>0.59611530000000001</v>
-      </c>
-      <c r="E13">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>122</v>
-      </c>
-      <c r="B14">
-        <v>2.6666669999999999</v>
-      </c>
-      <c r="C14">
-        <v>30</v>
-      </c>
-      <c r="D14" s="14">
-        <v>0.7488129</v>
-      </c>
-      <c r="E14">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>123</v>
-      </c>
-      <c r="B15">
-        <v>1.3461540000000001</v>
-      </c>
-      <c r="C15">
-        <v>26</v>
-      </c>
-      <c r="D15" s="14">
-        <v>1.5456369999999998E-8</v>
-      </c>
-      <c r="E15">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16">
-        <v>4.5333329999999998</v>
-      </c>
-      <c r="C16">
-        <v>30</v>
-      </c>
-      <c r="D16" s="14">
-        <v>0.9284559</v>
-      </c>
-      <c r="E16">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>125</v>
-      </c>
-      <c r="B17">
-        <v>1.125</v>
-      </c>
-      <c r="C17">
-        <v>8</v>
-      </c>
-      <c r="D17" s="14">
-        <v>5.1935330000000002E-17</v>
-      </c>
-      <c r="E17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>126</v>
-      </c>
-      <c r="B18">
-        <v>2.2083330000000001</v>
-      </c>
-      <c r="C18">
-        <v>24</v>
-      </c>
-      <c r="D18" s="14">
-        <v>1.60154E-9</v>
-      </c>
-      <c r="E18">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>127</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>6</v>
-      </c>
-      <c r="D19" s="14">
-        <v>5.5535569999999998E-46</v>
-      </c>
-      <c r="E19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>128</v>
-      </c>
-      <c r="B20">
-        <v>1.75</v>
-      </c>
-      <c r="C20">
-        <v>16</v>
-      </c>
-      <c r="D20" s="14">
-        <v>4.8449940000000001E-8</v>
-      </c>
-      <c r="E20">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>129</v>
-      </c>
-      <c r="B21">
-        <v>14.666667</v>
-      </c>
-      <c r="C21">
-        <v>30</v>
-      </c>
-      <c r="D21" s="14">
-        <v>0.93287909999999996</v>
-      </c>
-      <c r="E21">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>130</v>
-      </c>
-      <c r="B22">
-        <v>16</v>
-      </c>
-      <c r="C22">
-        <v>30</v>
-      </c>
-      <c r="D22" s="14">
-        <v>0.94018210000000002</v>
-      </c>
-      <c r="E22">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>131</v>
-      </c>
-      <c r="B23">
-        <v>1.230769</v>
-      </c>
-      <c r="C23">
-        <v>26</v>
-      </c>
-      <c r="D23" s="14">
-        <v>2.692315E-8</v>
-      </c>
-      <c r="E23">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>132</v>
-      </c>
-      <c r="B24">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="C24">
-        <v>30</v>
-      </c>
-      <c r="D24" s="14">
-        <v>0.97127980000000003</v>
-      </c>
-      <c r="E24">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{761263C3-34BE-4565-ADD5-D3E7F671F109}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:E25"/>
@@ -17561,13 +17168,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD0E3AA-364E-47AC-9DB2-92971155038C}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17787,70 +17394,377 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2C3236-CC60-4056-AE25-CF70CF1F3D8B}">
-  <dimension ref="A7:S37"/>
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="C12" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.44140625" customWidth="1"/>
+    <col min="16" max="16" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H1" t="s">
+        <v>190</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
+        <v>192</v>
+      </c>
+      <c r="M1" t="s">
+        <v>193</v>
+      </c>
+      <c r="N1" t="s">
+        <v>194</v>
+      </c>
+      <c r="O1" t="s">
+        <v>195</v>
+      </c>
+      <c r="P1" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>197</v>
+      </c>
+      <c r="R1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" s="13">
+        <v>25569.073645833334</v>
+      </c>
+      <c r="E2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G2" t="s">
+        <v>202</v>
+      </c>
+      <c r="H2" t="s">
+        <v>203</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="J2" s="13">
+        <v>25569.073622685184</v>
+      </c>
+      <c r="K2" s="20">
+        <v>1</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="M2" t="s">
+        <v>206</v>
+      </c>
+      <c r="N2">
+        <v>9</v>
+      </c>
+      <c r="P2" t="s">
+        <v>207</v>
+      </c>
+      <c r="R2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D3" s="13">
+        <v>25569.073657407407</v>
+      </c>
+      <c r="E3" t="s">
+        <v>200</v>
+      </c>
+      <c r="G3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H3" t="s">
+        <v>203</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="J3" s="13">
+        <v>25569.073622685184</v>
+      </c>
+      <c r="K3" s="20">
+        <v>1</v>
+      </c>
+      <c r="L3" s="21"/>
+      <c r="O3" t="s">
+        <v>211</v>
+      </c>
+      <c r="P3" t="s">
+        <v>212</v>
+      </c>
+      <c r="R3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D4" s="13">
+        <v>25569.073680555557</v>
+      </c>
+      <c r="E4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F4" t="s">
+        <v>201</v>
+      </c>
+      <c r="G4" t="s">
+        <v>202</v>
+      </c>
+      <c r="H4" t="s">
+        <v>203</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="J4" s="13">
+        <v>25569.073622685184</v>
+      </c>
+      <c r="K4" s="20">
+        <v>1</v>
+      </c>
+      <c r="L4" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="M4" t="s">
+        <v>206</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="P4" t="s">
+        <v>215</v>
+      </c>
+      <c r="R4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D5" s="13">
+        <v>25569.073703703703</v>
+      </c>
+      <c r="E5" t="s">
+        <v>200</v>
+      </c>
+      <c r="F5" t="s">
+        <v>201</v>
+      </c>
+      <c r="G5" t="s">
+        <v>202</v>
+      </c>
+      <c r="H5" t="s">
+        <v>203</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="J5" s="13">
+        <v>25569.073622685184</v>
+      </c>
+      <c r="K5" s="20">
+        <v>3</v>
+      </c>
+      <c r="L5" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="M5" t="s">
+        <v>218</v>
+      </c>
+      <c r="N5">
+        <v>-1</v>
+      </c>
+      <c r="O5" t="s">
+        <v>219</v>
+      </c>
+      <c r="P5" t="s">
+        <v>207</v>
+      </c>
+      <c r="R5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D6" s="13">
+        <v>25569.073715277777</v>
+      </c>
+      <c r="E6" t="s">
+        <v>200</v>
+      </c>
+      <c r="G6" t="s">
+        <v>210</v>
+      </c>
+      <c r="H6" t="s">
+        <v>203</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="J6" s="13">
+        <v>25569.073622685184</v>
+      </c>
+      <c r="K6" s="20">
+        <v>3</v>
+      </c>
+      <c r="L6" s="21"/>
+      <c r="O6" t="s">
+        <v>221</v>
+      </c>
+      <c r="P6" t="s">
+        <v>212</v>
+      </c>
+      <c r="R6" t="s">
+        <v>208</v>
+      </c>
+    </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="C7" t="s">
-        <v>185</v>
-      </c>
-      <c r="D7" t="s">
-        <v>186</v>
+        <v>222</v>
+      </c>
+      <c r="D7" s="13">
+        <v>25569.073738425926</v>
       </c>
       <c r="E7" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="F7" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="G7" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="H7" t="s">
-        <v>190</v>
-      </c>
-      <c r="I7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J7" t="s">
-        <v>191</v>
-      </c>
-      <c r="K7" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" t="s">
-        <v>192</v>
+        <v>203</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="J7" s="13">
+        <v>25569.073622685184</v>
+      </c>
+      <c r="K7" s="20">
+        <v>3</v>
+      </c>
+      <c r="L7" s="21" t="s">
+        <v>223</v>
       </c>
       <c r="M7" t="s">
-        <v>193</v>
-      </c>
-      <c r="N7" t="s">
-        <v>194</v>
-      </c>
-      <c r="O7" t="s">
-        <v>195</v>
+        <v>206</v>
+      </c>
+      <c r="N7">
+        <v>6</v>
       </c>
       <c r="P7" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="R7" t="s">
-        <v>45</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -17861,10 +17775,10 @@
         <v>198</v>
       </c>
       <c r="C8" t="s">
-        <v>199</v>
+        <v>224</v>
       </c>
       <c r="D8" s="13">
-        <v>25569.073645833334</v>
+        <v>25569.073761574073</v>
       </c>
       <c r="E8" t="s">
         <v>200</v>
@@ -17878,26 +17792,26 @@
       <c r="H8" t="s">
         <v>203</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="19" t="s">
         <v>204</v>
       </c>
       <c r="J8" s="13">
         <v>25569.073622685184</v>
       </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8" t="s">
-        <v>205</v>
+      <c r="K8" s="20">
+        <v>11</v>
+      </c>
+      <c r="L8" s="21" t="s">
+        <v>217</v>
       </c>
       <c r="M8" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="N8">
-        <v>9</v>
+        <v>-1</v>
       </c>
       <c r="P8" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="R8" t="s">
         <v>208</v>
@@ -17910,11 +17824,11 @@
       <c r="B9" t="s">
         <v>198</v>
       </c>
-      <c r="C9" t="s">
-        <v>209</v>
+      <c r="C9" s="14" t="s">
+        <v>225</v>
       </c>
       <c r="D9" s="13">
-        <v>25569.073657407407</v>
+        <v>25569.074467592593</v>
       </c>
       <c r="E9" t="s">
         <v>200</v>
@@ -17925,17 +17839,18 @@
       <c r="H9" t="s">
         <v>203</v>
       </c>
-      <c r="I9" t="s">
-        <v>204</v>
+      <c r="I9" s="19" t="s">
+        <v>226</v>
       </c>
       <c r="J9" s="13">
-        <v>25569.073622685184</v>
-      </c>
-      <c r="K9">
+        <v>25569.074456018519</v>
+      </c>
+      <c r="K9" s="20">
         <v>1</v>
       </c>
+      <c r="L9" s="21"/>
       <c r="O9" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="P9" t="s">
         <v>212</v>
@@ -17952,10 +17867,10 @@
         <v>198</v>
       </c>
       <c r="C10" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="D10" s="13">
-        <v>25569.073680555557</v>
+        <v>25569.074490740742</v>
       </c>
       <c r="E10" t="s">
         <v>200</v>
@@ -17969,23 +17884,23 @@
       <c r="H10" t="s">
         <v>203</v>
       </c>
-      <c r="I10" t="s">
-        <v>204</v>
+      <c r="I10" s="19" t="s">
+        <v>226</v>
       </c>
       <c r="J10" s="13">
-        <v>25569.073622685184</v>
-      </c>
-      <c r="K10">
+        <v>25569.074456018519</v>
+      </c>
+      <c r="K10" s="20">
         <v>1</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="21" t="s">
         <v>214</v>
       </c>
       <c r="M10" t="s">
         <v>206</v>
       </c>
       <c r="N10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P10" t="s">
         <v>215</v>
@@ -18002,10 +17917,10 @@
         <v>198</v>
       </c>
       <c r="C11" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="D11" s="13">
-        <v>25569.073703703703</v>
+        <v>25569.074513888889</v>
       </c>
       <c r="E11" t="s">
         <v>200</v>
@@ -18019,26 +17934,23 @@
       <c r="H11" t="s">
         <v>203</v>
       </c>
-      <c r="I11" t="s">
-        <v>204</v>
+      <c r="I11" s="19" t="s">
+        <v>226</v>
       </c>
       <c r="J11" s="13">
-        <v>25569.073622685184</v>
-      </c>
-      <c r="K11">
+        <v>25569.074456018519</v>
+      </c>
+      <c r="K11" s="20">
         <v>3</v>
       </c>
-      <c r="L11" t="s">
-        <v>217</v>
+      <c r="L11" s="21" t="s">
+        <v>230</v>
       </c>
       <c r="M11" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="N11">
-        <v>-1</v>
-      </c>
-      <c r="O11" t="s">
-        <v>219</v>
+        <v>2</v>
       </c>
       <c r="P11" t="s">
         <v>207</v>
@@ -18055,34 +17967,43 @@
         <v>198</v>
       </c>
       <c r="C12" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="D12" s="13">
-        <v>25569.073715277777</v>
+        <v>25569.074537037039</v>
       </c>
       <c r="E12" t="s">
         <v>200</v>
       </c>
+      <c r="F12" t="s">
+        <v>201</v>
+      </c>
       <c r="G12" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="H12" t="s">
         <v>203</v>
       </c>
-      <c r="I12" t="s">
-        <v>204</v>
+      <c r="I12" s="19" t="s">
+        <v>226</v>
       </c>
       <c r="J12" s="13">
-        <v>25569.073622685184</v>
-      </c>
-      <c r="K12">
+        <v>25569.074456018519</v>
+      </c>
+      <c r="K12" s="20">
         <v>3</v>
       </c>
-      <c r="O12" t="s">
-        <v>221</v>
+      <c r="L12" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="M12" t="s">
+        <v>206</v>
+      </c>
+      <c r="N12">
+        <v>2</v>
       </c>
       <c r="P12" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="R12" t="s">
         <v>208</v>
@@ -18096,43 +18017,35 @@
         <v>198</v>
       </c>
       <c r="C13" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="D13" s="13">
-        <v>25569.073738425926</v>
+        <v>25569.074548611112</v>
       </c>
       <c r="E13" t="s">
         <v>200</v>
       </c>
-      <c r="F13" t="s">
-        <v>201</v>
-      </c>
       <c r="G13" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="H13" t="s">
         <v>203</v>
       </c>
-      <c r="I13" t="s">
-        <v>204</v>
+      <c r="I13" s="19" t="s">
+        <v>226</v>
       </c>
       <c r="J13" s="13">
-        <v>25569.073622685184</v>
-      </c>
-      <c r="K13">
+        <v>25569.074456018519</v>
+      </c>
+      <c r="K13" s="20">
         <v>3</v>
       </c>
-      <c r="L13" t="s">
-        <v>223</v>
-      </c>
-      <c r="M13" t="s">
-        <v>206</v>
-      </c>
-      <c r="N13">
-        <v>6</v>
+      <c r="L13" s="21"/>
+      <c r="O13" t="s">
+        <v>233</v>
       </c>
       <c r="P13" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="R13" t="s">
         <v>208</v>
@@ -18146,10 +18059,10 @@
         <v>198</v>
       </c>
       <c r="C14" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="D14" s="13">
-        <v>25569.073761574073</v>
+        <v>25569.074571759258</v>
       </c>
       <c r="E14" t="s">
         <v>200</v>
@@ -18163,23 +18076,23 @@
       <c r="H14" t="s">
         <v>203</v>
       </c>
-      <c r="I14" t="s">
-        <v>204</v>
+      <c r="I14" s="19" t="s">
+        <v>226</v>
       </c>
       <c r="J14" s="13">
-        <v>25569.073622685184</v>
-      </c>
-      <c r="K14">
-        <v>11</v>
-      </c>
-      <c r="L14" t="s">
-        <v>217</v>
+        <v>25569.074456018519</v>
+      </c>
+      <c r="K14" s="20">
+        <v>3</v>
+      </c>
+      <c r="L14" s="21" t="s">
+        <v>223</v>
       </c>
       <c r="M14" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="N14">
-        <v>-1</v>
+        <v>14</v>
       </c>
       <c r="P14" t="s">
         <v>215</v>
@@ -18195,35 +18108,44 @@
       <c r="B15" t="s">
         <v>198</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>225</v>
+      <c r="C15" t="s">
+        <v>235</v>
       </c>
       <c r="D15" s="13">
-        <v>25569.074467592593</v>
+        <v>25569.074594907408</v>
       </c>
       <c r="E15" t="s">
         <v>200</v>
       </c>
+      <c r="F15" t="s">
+        <v>201</v>
+      </c>
       <c r="G15" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="H15" t="s">
         <v>203</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="19" t="s">
         <v>226</v>
       </c>
       <c r="J15" s="13">
         <v>25569.074456018519</v>
       </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="O15" t="s">
-        <v>227</v>
+      <c r="K15" s="20">
+        <v>11</v>
+      </c>
+      <c r="L15" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="M15" t="s">
+        <v>218</v>
+      </c>
+      <c r="N15">
+        <v>-1</v>
       </c>
       <c r="P15" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R15" t="s">
         <v>208</v>
@@ -18237,10 +18159,10 @@
         <v>198</v>
       </c>
       <c r="C16" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="D16" s="13">
-        <v>25569.074490740742</v>
+        <v>25569.074756944443</v>
       </c>
       <c r="E16" t="s">
         <v>200</v>
@@ -18254,23 +18176,23 @@
       <c r="H16" t="s">
         <v>203</v>
       </c>
-      <c r="I16" t="s">
-        <v>226</v>
+      <c r="I16" s="19" t="s">
+        <v>237</v>
       </c>
       <c r="J16" s="13">
-        <v>25569.074456018519</v>
-      </c>
-      <c r="K16">
+        <v>25569.074733796297</v>
+      </c>
+      <c r="K16" s="20">
         <v>1</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="21" t="s">
         <v>214</v>
       </c>
       <c r="M16" t="s">
         <v>206</v>
       </c>
       <c r="N16">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="P16" t="s">
         <v>215</v>
@@ -18287,10 +18209,10 @@
         <v>198</v>
       </c>
       <c r="C17" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="D17" s="13">
-        <v>25569.074513888889</v>
+        <v>25569.074780092593</v>
       </c>
       <c r="E17" t="s">
         <v>200</v>
@@ -18304,23 +18226,23 @@
       <c r="H17" t="s">
         <v>203</v>
       </c>
-      <c r="I17" t="s">
-        <v>226</v>
+      <c r="I17" s="19" t="s">
+        <v>237</v>
       </c>
       <c r="J17" s="13">
-        <v>25569.074456018519</v>
-      </c>
-      <c r="K17">
+        <v>25569.074733796297</v>
+      </c>
+      <c r="K17" s="20">
         <v>3</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" s="21" t="s">
         <v>230</v>
       </c>
       <c r="M17" t="s">
         <v>206</v>
       </c>
       <c r="N17">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="P17" t="s">
         <v>207</v>
@@ -18337,10 +18259,10 @@
         <v>198</v>
       </c>
       <c r="C18" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="D18" s="13">
-        <v>25569.074537037039</v>
+        <v>25569.074803240739</v>
       </c>
       <c r="E18" t="s">
         <v>200</v>
@@ -18354,26 +18276,26 @@
       <c r="H18" t="s">
         <v>203</v>
       </c>
-      <c r="I18" t="s">
-        <v>226</v>
+      <c r="I18" s="19" t="s">
+        <v>237</v>
       </c>
       <c r="J18" s="13">
-        <v>25569.074456018519</v>
-      </c>
-      <c r="K18">
+        <v>25569.074733796297</v>
+      </c>
+      <c r="K18" s="20">
         <v>3</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L18" s="21" t="s">
         <v>223</v>
       </c>
       <c r="M18" t="s">
         <v>206</v>
       </c>
       <c r="N18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="P18" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="R18" t="s">
         <v>208</v>
@@ -18387,484 +18309,547 @@
         <v>198</v>
       </c>
       <c r="C19" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="D19" s="13">
-        <v>25569.074548611112</v>
+        <v>25569.074826388889</v>
       </c>
       <c r="E19" t="s">
         <v>200</v>
       </c>
+      <c r="F19" t="s">
+        <v>201</v>
+      </c>
       <c r="G19" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="H19" t="s">
         <v>203</v>
       </c>
-      <c r="I19" t="s">
-        <v>226</v>
+      <c r="I19" s="19" t="s">
+        <v>237</v>
       </c>
       <c r="J19" s="13">
-        <v>25569.074456018519</v>
-      </c>
-      <c r="K19">
-        <v>3</v>
-      </c>
-      <c r="O19" t="s">
-        <v>233</v>
+        <v>25569.074733796297</v>
+      </c>
+      <c r="K19" s="20">
+        <v>11</v>
+      </c>
+      <c r="L19" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="M19" t="s">
+        <v>218</v>
+      </c>
+      <c r="N19">
+        <v>-1</v>
       </c>
       <c r="P19" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="R19" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" t="s">
-        <v>198</v>
-      </c>
-      <c r="C20" t="s">
-        <v>234</v>
-      </c>
-      <c r="D20" s="13">
-        <v>25569.074571759258</v>
-      </c>
-      <c r="E20" t="s">
-        <v>200</v>
-      </c>
-      <c r="F20" t="s">
-        <v>201</v>
-      </c>
-      <c r="G20" t="s">
-        <v>202</v>
-      </c>
-      <c r="H20" t="s">
-        <v>203</v>
-      </c>
-      <c r="I20" t="s">
-        <v>226</v>
-      </c>
-      <c r="J20" s="13">
-        <v>25569.074456018519</v>
-      </c>
-      <c r="K20">
-        <v>3</v>
-      </c>
-      <c r="L20" t="s">
-        <v>223</v>
-      </c>
-      <c r="M20" t="s">
-        <v>206</v>
-      </c>
-      <c r="N20">
-        <v>14</v>
-      </c>
-      <c r="P20" t="s">
-        <v>215</v>
-      </c>
-      <c r="R20" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" t="s">
-        <v>198</v>
-      </c>
-      <c r="C21" t="s">
-        <v>235</v>
-      </c>
-      <c r="D21" s="13">
-        <v>25569.074594907408</v>
-      </c>
-      <c r="E21" t="s">
-        <v>200</v>
-      </c>
-      <c r="F21" t="s">
-        <v>201</v>
-      </c>
-      <c r="G21" t="s">
-        <v>202</v>
-      </c>
-      <c r="H21" t="s">
-        <v>203</v>
-      </c>
-      <c r="I21" t="s">
-        <v>226</v>
-      </c>
-      <c r="J21" s="13">
-        <v>25569.074456018519</v>
-      </c>
-      <c r="K21">
-        <v>11</v>
-      </c>
-      <c r="L21" t="s">
-        <v>217</v>
-      </c>
-      <c r="M21" t="s">
-        <v>218</v>
-      </c>
-      <c r="N21">
-        <v>-1</v>
-      </c>
-      <c r="P21" t="s">
-        <v>215</v>
-      </c>
-      <c r="R21" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>198</v>
+        <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>236</v>
-      </c>
-      <c r="D22" s="13">
-        <v>25569.074756944443</v>
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
+        <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>200</v>
+        <v>34</v>
       </c>
       <c r="F22" t="s">
-        <v>201</v>
+        <v>35</v>
       </c>
       <c r="G22" t="s">
-        <v>202</v>
+        <v>36</v>
       </c>
       <c r="H22" t="s">
-        <v>203</v>
+        <v>37</v>
       </c>
       <c r="I22" t="s">
-        <v>237</v>
-      </c>
-      <c r="J22" s="13">
-        <v>25569.074733796297</v>
-      </c>
-      <c r="K22">
-        <v>1</v>
+        <v>38</v>
+      </c>
+      <c r="J22" t="s">
+        <v>39</v>
+      </c>
+      <c r="K22" t="s">
+        <v>40</v>
       </c>
       <c r="L22" t="s">
-        <v>214</v>
+        <v>41</v>
       </c>
       <c r="M22" t="s">
-        <v>206</v>
-      </c>
-      <c r="N22">
-        <v>9</v>
+        <v>42</v>
+      </c>
+      <c r="N22" t="s">
+        <v>47</v>
+      </c>
+      <c r="O22" t="s">
+        <v>48</v>
       </c>
       <c r="P22" t="s">
-        <v>215</v>
+        <v>43</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>44</v>
       </c>
       <c r="R22" t="s">
-        <v>208</v>
+        <v>45</v>
+      </c>
+      <c r="S22" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
         <v>11</v>
       </c>
-      <c r="B23" t="s">
-        <v>198</v>
-      </c>
-      <c r="C23" t="s">
-        <v>238</v>
-      </c>
-      <c r="D23" s="13">
-        <v>25569.074780092593</v>
-      </c>
-      <c r="E23" t="s">
-        <v>200</v>
-      </c>
-      <c r="F23" t="s">
-        <v>201</v>
-      </c>
-      <c r="G23" t="s">
-        <v>202</v>
-      </c>
-      <c r="H23" t="s">
-        <v>203</v>
-      </c>
-      <c r="I23" t="s">
-        <v>237</v>
-      </c>
-      <c r="J23" s="13">
-        <v>25569.074733796297</v>
+      <c r="C23" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="20">
+        <v>1</v>
+      </c>
+      <c r="F23" s="13">
+        <v>25569.073611111111</v>
+      </c>
+      <c r="G23" s="13">
+        <v>25569.073611111111</v>
+      </c>
+      <c r="H23" s="13">
+        <v>25569.073611111111</v>
+      </c>
+      <c r="I23" s="13">
+        <v>25569.073611111111</v>
+      </c>
+      <c r="J23" t="s">
+        <v>241</v>
       </c>
       <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="O23">
         <v>3</v>
       </c>
-      <c r="L23" t="s">
-        <v>230</v>
-      </c>
-      <c r="M23" t="s">
-        <v>206</v>
-      </c>
-      <c r="N23">
-        <v>9</v>
-      </c>
       <c r="P23" t="s">
-        <v>207</v>
+        <v>118</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
       </c>
       <c r="R23" t="s">
         <v>208</v>
       </c>
+      <c r="S23">
+        <v>36</v>
+      </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
         <v>11</v>
       </c>
-      <c r="B24" t="s">
-        <v>198</v>
-      </c>
-      <c r="C24" t="s">
-        <v>239</v>
-      </c>
-      <c r="D24" s="13">
-        <v>25569.074803240739</v>
-      </c>
-      <c r="E24" t="s">
-        <v>200</v>
-      </c>
-      <c r="F24" t="s">
-        <v>201</v>
-      </c>
-      <c r="G24" t="s">
-        <v>202</v>
-      </c>
-      <c r="H24" t="s">
-        <v>203</v>
-      </c>
-      <c r="I24" t="s">
-        <v>237</v>
-      </c>
-      <c r="J24" s="13">
-        <v>25569.074733796297</v>
+      <c r="C24" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" s="20">
+        <v>3</v>
+      </c>
+      <c r="F24" s="13">
+        <v>25569.073611111111</v>
+      </c>
+      <c r="G24" s="13">
+        <v>25569.073611111111</v>
+      </c>
+      <c r="H24" s="13">
+        <v>25569.073611111111</v>
+      </c>
+      <c r="I24" s="13">
+        <v>25569.073611111111</v>
+      </c>
+      <c r="J24" t="s">
+        <v>241</v>
       </c>
       <c r="K24">
-        <v>3</v>
-      </c>
-      <c r="L24" t="s">
-        <v>223</v>
-      </c>
-      <c r="M24" t="s">
-        <v>206</v>
-      </c>
-      <c r="N24">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="O24">
+        <v>11</v>
       </c>
       <c r="P24" t="s">
-        <v>215</v>
+        <v>124</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
       </c>
       <c r="R24" t="s">
         <v>208</v>
       </c>
+      <c r="S24">
+        <v>37</v>
+      </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25">
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
         <v>11</v>
       </c>
-      <c r="B25" t="s">
-        <v>198</v>
-      </c>
-      <c r="C25" t="s">
-        <v>240</v>
-      </c>
-      <c r="D25" s="13">
-        <v>25569.074826388889</v>
-      </c>
-      <c r="E25" t="s">
-        <v>200</v>
-      </c>
-      <c r="F25" t="s">
-        <v>201</v>
-      </c>
-      <c r="G25" t="s">
-        <v>202</v>
-      </c>
-      <c r="H25" t="s">
-        <v>203</v>
-      </c>
-      <c r="I25" t="s">
-        <v>237</v>
-      </c>
-      <c r="J25" s="13">
-        <v>25569.074733796297</v>
+      <c r="C25" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="20">
+        <v>11</v>
+      </c>
+      <c r="F25" s="13">
+        <v>25569.073611111111</v>
+      </c>
+      <c r="G25" s="13">
+        <v>25569.073611111111</v>
+      </c>
+      <c r="H25" s="13">
+        <v>25569.073611111111</v>
+      </c>
+      <c r="I25" s="13">
+        <v>25569.073611111111</v>
+      </c>
+      <c r="J25" t="s">
+        <v>242</v>
       </c>
       <c r="K25">
-        <v>11</v>
-      </c>
-      <c r="L25" t="s">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="M25" t="s">
-        <v>218</v>
-      </c>
-      <c r="N25">
-        <v>-1</v>
+      <c r="O25">
+        <v>12</v>
       </c>
       <c r="P25" t="s">
-        <v>215</v>
+        <v>124</v>
+      </c>
+      <c r="Q25">
+        <v>2</v>
       </c>
       <c r="R25" t="s">
         <v>208</v>
       </c>
+      <c r="S25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="20">
+        <v>1</v>
+      </c>
+      <c r="F26" s="13">
+        <v>25569.074305555554</v>
+      </c>
+      <c r="G26" s="13">
+        <v>25569.074305555554</v>
+      </c>
+      <c r="H26" s="13">
+        <v>25569.074305555554</v>
+      </c>
+      <c r="I26" s="13">
+        <v>25569.074305555554</v>
+      </c>
+      <c r="J26" t="s">
+        <v>243</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="O26">
+        <v>16</v>
+      </c>
+      <c r="P26" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="R26" t="s">
+        <v>208</v>
+      </c>
+      <c r="S26">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="20">
+        <v>3</v>
+      </c>
+      <c r="F27" s="13">
+        <v>25569.074305555554</v>
+      </c>
+      <c r="G27" s="13">
+        <v>25569.074305555554</v>
+      </c>
+      <c r="H27" s="13">
+        <v>25569.074305555554</v>
+      </c>
+      <c r="I27" s="13">
+        <v>25569.074305555554</v>
+      </c>
+      <c r="J27" t="s">
+        <v>241</v>
+      </c>
+      <c r="K27">
+        <v>2</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+      <c r="R27" t="s">
+        <v>208</v>
+      </c>
+      <c r="S27">
+        <v>58</v>
+      </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>31</v>
+      <c r="A28">
+        <v>59</v>
       </c>
       <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" s="20">
+        <v>11</v>
+      </c>
+      <c r="F28" s="13">
+        <v>25569.074305555554</v>
+      </c>
+      <c r="G28" s="13">
+        <v>25569.074305555554</v>
+      </c>
+      <c r="H28" s="13">
+        <v>25569.074305555554</v>
+      </c>
+      <c r="I28" s="13">
+        <v>25569.074305555554</v>
+      </c>
+      <c r="J28" t="s">
+        <v>242</v>
+      </c>
+      <c r="K28">
         <v>0</v>
       </c>
-      <c r="C28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" t="s">
-        <v>34</v>
-      </c>
-      <c r="F28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G28" t="s">
-        <v>36</v>
-      </c>
-      <c r="H28" t="s">
-        <v>37</v>
-      </c>
-      <c r="I28" t="s">
-        <v>38</v>
-      </c>
-      <c r="J28" t="s">
-        <v>39</v>
-      </c>
-      <c r="K28" t="s">
-        <v>40</v>
-      </c>
-      <c r="L28" t="s">
-        <v>41</v>
-      </c>
-      <c r="M28" t="s">
-        <v>42</v>
-      </c>
-      <c r="N28" t="s">
-        <v>47</v>
-      </c>
-      <c r="O28" t="s">
-        <v>48</v>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="O28">
+        <v>17</v>
       </c>
       <c r="P28" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>44</v>
+        <v>124</v>
+      </c>
+      <c r="Q28">
+        <v>3</v>
       </c>
       <c r="R28" t="s">
-        <v>45</v>
-      </c>
-      <c r="S28" t="s">
-        <v>46</v>
+        <v>208</v>
+      </c>
+      <c r="S28">
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
       </c>
-      <c r="C29" t="s">
-        <v>204</v>
+      <c r="C29" s="19" t="s">
+        <v>237</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="20">
         <v>1</v>
       </c>
       <c r="F29" s="13">
-        <v>25569.073611111111</v>
+        <v>25569.074305555554</v>
       </c>
       <c r="G29" s="13">
-        <v>25569.073611111111</v>
+        <v>25569.074305555554</v>
       </c>
       <c r="H29" s="13">
-        <v>25569.073611111111</v>
+        <v>25569.074305555554</v>
       </c>
       <c r="I29" s="13">
-        <v>25569.073611111111</v>
+        <v>25569.074305555554</v>
       </c>
       <c r="J29" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="K29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L29">
         <v>1</v>
       </c>
       <c r="M29">
-        <v>1</v>
-      </c>
-      <c r="N29" t="s">
-        <v>205</v>
+        <v>0</v>
+      </c>
+      <c r="N29" s="21" t="s">
+        <v>214</v>
       </c>
       <c r="O29">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="P29" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="Q29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R29" t="s">
         <v>208</v>
       </c>
       <c r="S29">
-        <v>36</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
       </c>
-      <c r="C30" t="s">
-        <v>204</v>
+      <c r="C30" s="19" t="s">
+        <v>237</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="20">
         <v>3</v>
       </c>
       <c r="F30" s="13">
-        <v>25569.073611111111</v>
+        <v>25569.074305555554</v>
       </c>
       <c r="G30" s="13">
-        <v>25569.073611111111</v>
+        <v>25569.074305555554</v>
       </c>
       <c r="H30" s="13">
-        <v>25569.073611111111</v>
+        <v>25569.074305555554</v>
       </c>
       <c r="I30" s="13">
-        <v>25569.073611111111</v>
+        <v>25569.074305555554</v>
       </c>
       <c r="J30" t="s">
         <v>241</v>
@@ -18876,54 +18861,54 @@
         <v>1</v>
       </c>
       <c r="M30">
-        <v>1</v>
-      </c>
-      <c r="N30" t="s">
-        <v>217</v>
+        <v>0</v>
+      </c>
+      <c r="N30" s="21" t="s">
+        <v>230</v>
       </c>
       <c r="O30">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="P30" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="Q30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R30" t="s">
         <v>208</v>
       </c>
       <c r="S30">
-        <v>37</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
       </c>
-      <c r="C31" t="s">
-        <v>204</v>
+      <c r="C31" s="19" t="s">
+        <v>237</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="20">
         <v>11</v>
       </c>
       <c r="F31" s="13">
-        <v>25569.073611111111</v>
+        <v>25569.074305555554</v>
       </c>
       <c r="G31" s="13">
-        <v>25569.073611111111</v>
+        <v>25569.074305555554</v>
       </c>
       <c r="H31" s="13">
-        <v>25569.073611111111</v>
+        <v>25569.074305555554</v>
       </c>
       <c r="I31" s="13">
-        <v>25569.073611111111</v>
+        <v>25569.074305555554</v>
       </c>
       <c r="J31" t="s">
         <v>242</v>
@@ -18937,377 +18922,628 @@
       <c r="M31">
         <v>0</v>
       </c>
-      <c r="N31" t="s">
+      <c r="N31" s="21" t="s">
         <v>217</v>
       </c>
       <c r="O31">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="P31" t="s">
         <v>124</v>
       </c>
       <c r="Q31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R31" t="s">
         <v>208</v>
       </c>
       <c r="S31">
-        <v>38</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>57</v>
-      </c>
-      <c r="B32" t="s">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B37" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B38" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B39" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B40" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B41" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B42" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B43" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B44" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B45" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B46" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B47" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B48" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B49" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B50" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B51" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B52" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA8BBC2-48DE-43AF-A080-6B5302FDA786}">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="C32" t="s">
+      <c r="B2" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" s="20">
+        <v>1</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="E2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="G2" s="20">
+        <v>1</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="I2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C3" s="20">
+        <v>1</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="G3" s="20">
+        <v>3</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="I3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" s="20">
+        <v>1</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="E4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="G4" s="20">
+        <v>11</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="I4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C5" s="20">
+        <v>3</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="E5" t="s">
+        <v>207</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="D32">
+      <c r="G5" s="20">
         <v>1</v>
       </c>
-      <c r="E32">
+      <c r="H5" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="I5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C6" s="20">
+        <v>3</v>
+      </c>
+      <c r="D6" s="21"/>
+      <c r="E6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="G6" s="20">
+        <v>3</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="I6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C7" s="20">
+        <v>3</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="E7" t="s">
+        <v>215</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="G7" s="20">
+        <v>11</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="I7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C8" s="20">
+        <v>11</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="E8" t="s">
+        <v>215</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="G8" s="20">
         <v>1</v>
       </c>
-      <c r="F32" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="G32" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="H32" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="I32" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="J32" t="s">
-        <v>243</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-      <c r="L32">
+      <c r="H8" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="I8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C9" s="20">
         <v>1</v>
       </c>
-      <c r="M32">
+      <c r="D9" s="21"/>
+      <c r="E9" t="s">
+        <v>212</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="G9" s="20">
+        <v>3</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="I9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C10" s="20">
         <v>1</v>
       </c>
-      <c r="N32" t="s">
+      <c r="D10" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="O32">
-        <v>16</v>
-      </c>
-      <c r="P32" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q32">
+      <c r="E10" t="s">
+        <v>215</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="G10" s="20">
+        <v>11</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="I10" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C11" s="20">
+        <v>3</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="E11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C12" s="20">
+        <v>3</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="E12" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C13" s="20">
+        <v>3</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C14" s="20">
+        <v>3</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="E14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C15" s="20">
+        <v>11</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="E15" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="C16" s="20">
         <v>1</v>
       </c>
-      <c r="R32" t="s">
-        <v>208</v>
-      </c>
-      <c r="S32">
-        <v>57</v>
+      <c r="D16" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="E16" t="s">
+        <v>215</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>58</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="C33" t="s">
-        <v>226</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33">
+      <c r="B17" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="C17" s="20">
         <v>3</v>
       </c>
-      <c r="F33" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="G33" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="H33" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="I33" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="J33" t="s">
-        <v>241</v>
-      </c>
-      <c r="K33">
-        <v>2</v>
-      </c>
-      <c r="L33">
-        <v>1</v>
-      </c>
-      <c r="M33">
-        <v>1</v>
-      </c>
-      <c r="N33" t="s">
+      <c r="D17" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="O33">
-        <v>1</v>
-      </c>
-      <c r="P33" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q33">
-        <v>1</v>
-      </c>
-      <c r="R33" t="s">
-        <v>208</v>
-      </c>
-      <c r="S33">
-        <v>58</v>
+      <c r="E17" t="s">
+        <v>207</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>59</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>11</v>
       </c>
-      <c r="C34" t="s">
-        <v>226</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34">
+      <c r="B18" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="C18" s="20">
+        <v>3</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="E18" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="G34" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="H34" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="I34" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="J34" t="s">
-        <v>242</v>
-      </c>
-      <c r="K34">
-        <v>0</v>
-      </c>
-      <c r="L34">
-        <v>1</v>
-      </c>
-      <c r="M34">
-        <v>0</v>
-      </c>
-      <c r="N34" t="s">
+      <c r="B19" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="C19" s="20">
+        <v>11</v>
+      </c>
+      <c r="D19" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="O34">
-        <v>17</v>
-      </c>
-      <c r="P34" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q34">
-        <v>3</v>
-      </c>
-      <c r="R34" t="s">
-        <v>208</v>
-      </c>
-      <c r="S34">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>63</v>
-      </c>
-      <c r="B35" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" t="s">
-        <v>237</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="F35" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="G35" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="H35" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="I35" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="J35" t="s">
-        <v>242</v>
-      </c>
-      <c r="K35">
-        <v>0</v>
-      </c>
-      <c r="L35">
-        <v>1</v>
-      </c>
-      <c r="M35">
-        <v>0</v>
-      </c>
-      <c r="N35" t="s">
-        <v>214</v>
-      </c>
-      <c r="O35">
-        <v>18</v>
-      </c>
-      <c r="P35" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q35">
-        <v>2</v>
-      </c>
-      <c r="R35" t="s">
-        <v>208</v>
-      </c>
-      <c r="S35">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>64</v>
-      </c>
-      <c r="B36" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" t="s">
-        <v>237</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36">
-        <v>3</v>
-      </c>
-      <c r="F36" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="G36" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="H36" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="I36" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="J36" t="s">
-        <v>241</v>
-      </c>
-      <c r="K36">
-        <v>1</v>
-      </c>
-      <c r="L36">
-        <v>1</v>
-      </c>
-      <c r="M36">
-        <v>0</v>
-      </c>
-      <c r="N36" t="s">
-        <v>230</v>
-      </c>
-      <c r="O36">
-        <v>2</v>
-      </c>
-      <c r="P36" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q36">
-        <v>2</v>
-      </c>
-      <c r="R36" t="s">
-        <v>208</v>
-      </c>
-      <c r="S36">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>65</v>
-      </c>
-      <c r="B37" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" t="s">
-        <v>237</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37">
-        <v>11</v>
-      </c>
-      <c r="F37" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="G37" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="H37" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="I37" s="13">
-        <v>25569.074305555554</v>
-      </c>
-      <c r="J37" t="s">
-        <v>242</v>
-      </c>
-      <c r="K37">
-        <v>0</v>
-      </c>
-      <c r="L37">
-        <v>1</v>
-      </c>
-      <c r="M37">
-        <v>0</v>
-      </c>
-      <c r="N37" t="s">
-        <v>217</v>
-      </c>
-      <c r="O37">
-        <v>19</v>
-      </c>
-      <c r="P37" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q37">
-        <v>4</v>
-      </c>
-      <c r="R37" t="s">
-        <v>208</v>
-      </c>
-      <c r="S37">
-        <v>65</v>
+      <c r="E19" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>